<commit_message>
Regresa a sus páginas respectivas, con variaciones en sus nombres
</commit_message>
<xml_diff>
--- a/ClinicalSheet2_0/data/Documentos/Pacientes.xlsx
+++ b/ClinicalSheet2_0/data/Documentos/Pacientes.xlsx
@@ -98,6 +98,43 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Diana Alejandra</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Alvarado Sierra</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>51905677</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>07</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Agosto</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>1968</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>unmilagroenmividacadadia</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>